<commit_message>
Assignment three with extra credit
</commit_message>
<xml_diff>
--- a/AssignmentThree/RESTAURANT LIST.xlsx
+++ b/AssignmentThree/RESTAURANT LIST.xlsx
@@ -30,9 +30,6 @@
     <t>VA</t>
   </si>
   <si>
-    <t>https://www.google.com/url?sa=i&amp;rct=j&amp;q=&amp;esrc=s&amp;source=images&amp;cd=&amp;cad=rja&amp;uact=8&amp;ved=0ahUKEwjThsHG2NzUAhVBbT4KHTtKAyAQjRwIBw&amp;url=https%3A%2F%2Ffoursquare.com%2Fv%2Fsiam-classic%2F4b776a6af964a52001992ee3%2Fphotos&amp;psig=AFQjCNE3c_0T5SKaFM-5n6AZ9cOw8TU9AA&amp;ust=1498607074661760</t>
-  </si>
-  <si>
     <t>Matchbox One Loudon</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>https://www.google.com/maps/place/CRUST/@25.7785971,-80.2060641,3a,75y,90t/data=!3m8!1e2!3m6!1shttp:%2F%2Fstatic.urbandaddy.com%2Fuploads%2Fassets%2Fimage%2Fslideshows%2Fstandard%2F86ce6cbc06df0f3a40e74d14b46bef22.jpg!2e7!3e27!6s%2F%2Flh5.googleusercontent.com%2Fproxy%2FWubukWFywJDbuMEBI_pa0rBXLlUN4PdNM5tVLU6E86-Nlm9Jf4D7t6pMKYtrG5D8yq5adb7GD2t6dOWPhVZl-cg2K-wI7A1PawJO76GZYeOzmdTBylA8qfngLerKClTNuVF9RLbWf7ELiu5_np8_32aOjqJgVno%3Dw169-h106-k-no!7i728!8i456!4m5!3m4!1s0x88d9ab5daa626989:0x1178fd2db66e46cc!8m2!3d25.778432!4d-80.206048</t>
   </si>
   <si>
-    <t>Café Juanita</t>
-  </si>
-  <si>
     <t>9702 NE 120th Pl</t>
   </si>
   <si>
@@ -655,6 +649,12 @@
   </si>
   <si>
     <t>https://cdn0.vox-cdn.com/thumbor/bPQYYjUhWlKq5QN3TV64JTQ4dlQ=/0x25:500x306/1600x900/cdn0.vox-cdn.com/uploads/chorus_image/image/38814976/minibar500.0.jpg</t>
+  </si>
+  <si>
+    <t>https://igx.4sqi.net/img/general/width960/8sGgDH5FXm96ffYkM1wEmI59Ao0ITofSB-7jWINGJVc.jpg</t>
+  </si>
+  <si>
+    <t>Cafe Juanita</t>
   </si>
 </sst>
 </file>
@@ -662,8 +662,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
-    <numFmt numFmtId="166" formatCode="00000"/>
+    <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+    <numFmt numFmtId="165" formatCode="00000"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -772,27 +772,27 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1099,7 +1099,7 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1108,10 +1108,10 @@
     <col min="2" max="2" width="29.5546875" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="22.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="10" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
     <col min="7" max="7" width="14.88671875" customWidth="1"/>
-    <col min="8" max="8" width="15" style="11" customWidth="1"/>
+    <col min="8" max="8" width="15" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1127,7 +1127,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12">
+      <c r="E1" s="14">
         <v>20110</v>
       </c>
       <c r="F1" s="1">
@@ -1136,27 +1136,27 @@
       <c r="G1" s="1">
         <v>-77.472750500000004</v>
       </c>
-      <c r="H1" s="9">
+      <c r="H1" s="12">
         <v>7033685647</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>4</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="14">
         <v>20147</v>
       </c>
       <c r="F2" s="1">
@@ -1165,27 +1165,27 @@
       <c r="G2" s="1">
         <v>-77.453372000000002</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="12">
         <v>5719188024</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="14">
         <v>22003</v>
       </c>
       <c r="F3" s="1">
@@ -1194,27 +1194,27 @@
       <c r="G3" s="1">
         <v>-77.203422000000003</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="12">
         <v>7032562086</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="14">
         <v>22003</v>
       </c>
       <c r="F4" s="1">
@@ -1223,27 +1223,27 @@
       <c r="G4" s="1">
         <v>-77.206023999999999</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="12">
         <v>7037500775</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="14">
         <v>22003</v>
       </c>
       <c r="F5" s="1">
@@ -1252,27 +1252,27 @@
       <c r="G5" s="1">
         <v>-77.209868</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="12">
         <v>7039144646</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="12">
+      <c r="E6" s="14">
         <v>63010</v>
       </c>
       <c r="F6" s="1">
@@ -1281,27 +1281,27 @@
       <c r="G6" s="1">
         <v>-90.386505</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="12">
         <v>6364643200</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="14">
         <v>22003</v>
       </c>
       <c r="F7" s="1">
@@ -1310,27 +1310,27 @@
       <c r="G7" s="1">
         <v>-77.197413999999995</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="12">
         <v>7039145775</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="14">
         <v>22003</v>
       </c>
       <c r="F8" s="1">
@@ -1339,27 +1339,27 @@
       <c r="G8" s="1">
         <v>-77.210697999999994</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="12">
         <v>7034629093</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="12">
+        <v>21</v>
+      </c>
+      <c r="E9" s="14">
         <v>63103</v>
       </c>
       <c r="F9" s="1">
@@ -1368,27 +1368,27 @@
       <c r="G9" s="1">
         <v>-90.224029000000002</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="12">
         <v>3145354340</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="14">
         <v>22201</v>
       </c>
       <c r="F10" s="1">
@@ -1397,27 +1397,27 @@
       <c r="G10" s="1">
         <v>-77.096340999999995</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="12">
         <v>7036725395</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="12">
+      <c r="E11" s="14">
         <v>33131</v>
       </c>
       <c r="F11" s="1">
@@ -1426,27 +1426,27 @@
       <c r="G11" s="1">
         <v>-80.190128000000001</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="12">
         <v>3055770277</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="12">
+      <c r="E12" s="14">
         <v>33131</v>
       </c>
       <c r="F12" s="1">
@@ -1455,27 +1455,27 @@
       <c r="G12" s="1">
         <v>80.185160999999994</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="12">
         <v>3059138358</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="12">
+      <c r="E13" s="14">
         <v>33128</v>
       </c>
       <c r="F13" s="1">
@@ -1484,27 +1484,27 @@
       <c r="G13" s="1">
         <v>-80.211027000000001</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="12">
         <v>3053717065</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="12">
+      <c r="E14" s="14">
         <v>98034</v>
       </c>
       <c r="F14" s="1">
@@ -1513,27 +1513,27 @@
       <c r="G14" s="1">
         <v>-122.200968</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="12">
         <v>4258231505</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="12">
+        <v>50</v>
+      </c>
+      <c r="E15" s="14">
         <v>98022</v>
       </c>
       <c r="F15" s="1">
@@ -1542,27 +1542,27 @@
       <c r="G15" s="1">
         <v>-121.48349899999999</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="12">
         <v>3606633085</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="12">
+      <c r="E16" s="14">
         <v>20006</v>
       </c>
       <c r="F16" s="1">
@@ -1571,27 +1571,27 @@
       <c r="G16" s="1">
         <v>-77.044387</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="12">
         <v>2028228783</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="14">
         <v>22015</v>
       </c>
       <c r="F17" s="1">
@@ -1600,27 +1600,27 @@
       <c r="G17" s="1">
         <v>-77.273150999999999</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="12">
         <v>7037648882</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="12">
+        <v>21</v>
+      </c>
+      <c r="E18" s="14">
         <v>63118</v>
       </c>
       <c r="F18" s="1">
@@ -1629,27 +1629,27 @@
       <c r="G18" s="1">
         <v>-90.235952999999995</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="12">
         <v>3147761407</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="D19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="14">
         <v>22031</v>
       </c>
       <c r="F19" s="1">
@@ -1658,27 +1658,27 @@
       <c r="G19" s="1">
         <v>-77.230141000000003</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="12">
         <v>5713261616</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="12">
+        <v>21</v>
+      </c>
+      <c r="E20" s="14">
         <v>63130</v>
       </c>
       <c r="F20" s="1">
@@ -1687,27 +1687,27 @@
       <c r="G20" s="1">
         <v>-90.305074599999998</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="12">
         <v>3147270200</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="14">
         <v>22201</v>
       </c>
       <c r="F21" s="1">
@@ -1716,27 +1716,27 @@
       <c r="G21" s="1">
         <v>-77.097198000000006</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="12">
         <v>7038128600</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="14">
         <v>22003</v>
       </c>
       <c r="F22" s="1">
@@ -1745,27 +1745,27 @@
       <c r="G22" s="1">
         <v>-77.213562999999994</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="12">
         <v>7039428182</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="12">
+        <v>21</v>
+      </c>
+      <c r="E23" s="14">
         <v>63108</v>
       </c>
       <c r="F23" s="1">
@@ -1774,27 +1774,27 @@
       <c r="G23" s="1">
         <v>-90.260863999999998</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="12">
         <v>3149302955</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="D24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="12">
+        <v>21</v>
+      </c>
+      <c r="E24" s="14">
         <v>63052</v>
       </c>
       <c r="F24" s="1">
@@ -1803,27 +1803,27 @@
       <c r="G24" s="1">
         <v>-90.381264999999999</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="12">
         <v>6364648889</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" s="12">
+      <c r="E25" s="14">
         <v>97530</v>
       </c>
       <c r="F25" s="1">
@@ -1832,27 +1832,27 @@
       <c r="G25" s="1">
         <v>-122.96898</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="12">
         <v>5418994450</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="12">
+        <v>50</v>
+      </c>
+      <c r="E26" s="14">
         <v>98033</v>
       </c>
       <c r="F26" s="1">
@@ -1861,27 +1861,27 @@
       <c r="G26" s="1">
         <v>-122.20384799999999</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="12">
         <v>4252845900</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="D27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="14">
         <v>20190</v>
       </c>
       <c r="F27" s="1">
@@ -1890,27 +1890,27 @@
       <c r="G27" s="1">
         <v>-77.356530000000006</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="12">
         <v>7033188920</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="14">
         <v>20190</v>
       </c>
       <c r="F28" s="1">
@@ -1919,27 +1919,27 @@
       <c r="G28" s="1">
         <v>-77.359915000000001</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="12">
         <v>7032303474</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="D29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" s="12">
+        <v>21</v>
+      </c>
+      <c r="E29" s="14">
         <v>63012</v>
       </c>
       <c r="F29" s="1">
@@ -1948,27 +1948,27 @@
       <c r="G29" s="1">
         <v>-90.399951999999999</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="12">
         <v>6364640110</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="D30" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E30" s="12">
+        <v>50</v>
+      </c>
+      <c r="E30" s="14">
         <v>98402</v>
       </c>
       <c r="F30" s="1">
@@ -1977,27 +1977,27 @@
       <c r="G30" s="1">
         <v>-122.480733</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="12">
         <v>2537525444</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="14">
         <v>22031</v>
       </c>
       <c r="F31" s="1">
@@ -2006,27 +2006,27 @@
       <c r="G31" s="1">
         <v>-77.228780999999998</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="12">
         <v>7039927892</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="14">
         <v>22003</v>
       </c>
       <c r="F32" s="1">
@@ -2035,27 +2035,27 @@
       <c r="G32" s="1">
         <v>-77.205751000000006</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="12">
         <v>7039140594</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E33" s="12">
+      <c r="E33" s="14">
         <v>22031</v>
       </c>
       <c r="F33" s="1">
@@ -2064,27 +2064,27 @@
       <c r="G33" s="1">
         <v>-77.230359000000007</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H33" s="12">
         <v>7034629322</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E34" s="12">
+        <v>21</v>
+      </c>
+      <c r="E34" s="14">
         <v>63026</v>
       </c>
       <c r="F34" s="1">
@@ -2093,27 +2093,27 @@
       <c r="G34" s="1">
         <v>-90.443945999999997</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H34" s="12">
         <v>6363264006</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="D35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E35" s="12">
+      <c r="E35" s="14">
         <v>22042</v>
       </c>
       <c r="F35" s="1">
@@ -2122,27 +2122,27 @@
       <c r="G35" s="1">
         <v>-77.228244000000004</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H35" s="12">
         <v>7035398566</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="12">
+      <c r="E36" s="14">
         <v>22003</v>
       </c>
       <c r="F36" s="1">
@@ -2151,27 +2151,27 @@
       <c r="G36" s="1">
         <v>-77.210136000000006</v>
       </c>
-      <c r="H36" s="9">
+      <c r="H36" s="12">
         <v>7039413693</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="D37" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="12">
+      <c r="E37" s="14">
         <v>22102</v>
       </c>
       <c r="F37" s="1">
@@ -2180,27 +2180,27 @@
       <c r="G37" s="1">
         <v>-77.218115999999995</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H37" s="12">
         <v>7039428810</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E38" s="12">
+      <c r="E38" s="14">
         <v>22102</v>
       </c>
       <c r="F38" s="1">
@@ -2209,27 +2209,27 @@
       <c r="G38" s="1">
         <v>-77.219080000000005</v>
       </c>
-      <c r="H38" s="9">
+      <c r="H38" s="12">
         <v>7032883852</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="12">
+      <c r="E39" s="14">
         <v>22031</v>
       </c>
       <c r="F39" s="1">
@@ -2238,27 +2238,27 @@
       <c r="G39" s="1">
         <v>-77.229346000000007</v>
       </c>
-      <c r="H39" s="9">
+      <c r="H39" s="12">
         <v>7032800000</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="D40" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E40" s="12">
+      <c r="E40" s="14">
         <v>22150</v>
       </c>
       <c r="F40" s="1">
@@ -2267,27 +2267,27 @@
       <c r="G40" s="1">
         <v>-77.186149999999998</v>
       </c>
-      <c r="H40" s="9">
+      <c r="H40" s="12">
         <v>7036447100</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="12">
+      <c r="E41" s="14">
         <v>22150</v>
       </c>
       <c r="F41" s="1">
@@ -2296,27 +2296,27 @@
       <c r="G41" s="1">
         <v>-77.175202999999996</v>
       </c>
-      <c r="H41" s="9">
+      <c r="H41" s="12">
         <v>7039239309</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E42" s="12">
+      <c r="E42" s="14">
         <v>22205</v>
       </c>
       <c r="F42" s="1">
@@ -2325,27 +2325,27 @@
       <c r="G42" s="1">
         <v>-77.142266000000006</v>
       </c>
-      <c r="H42" s="9">
+      <c r="H42" s="12">
         <v>7032418681</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E43" s="12">
+      <c r="E43" s="14">
         <v>22202</v>
       </c>
       <c r="F43" s="1">
@@ -2354,27 +2354,27 @@
       <c r="G43" s="1">
         <v>-77.062862999999993</v>
       </c>
-      <c r="H43" s="9">
+      <c r="H43" s="12">
         <v>7034138200</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E44" s="12">
+      <c r="E44" s="14">
         <v>22201</v>
       </c>
       <c r="F44" s="1">
@@ -2383,27 +2383,27 @@
       <c r="G44" s="1">
         <v>-77.093243999999999</v>
       </c>
-      <c r="H44" s="9">
+      <c r="H44" s="12">
         <v>7032949966</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="12">
+      <c r="E45" s="14">
         <v>22207</v>
       </c>
       <c r="F45" s="1">
@@ -2412,27 +2412,27 @@
       <c r="G45" s="1">
         <v>-77.122900000000001</v>
       </c>
-      <c r="H45" s="9">
+      <c r="H45" s="12">
         <v>7035282464</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="D46" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E46" s="12">
+      <c r="E46" s="14">
         <v>22191</v>
       </c>
       <c r="F46" s="1">
@@ -2441,27 +2441,27 @@
       <c r="G46" s="1">
         <v>-77.287648000000004</v>
       </c>
-      <c r="H46" s="9">
+      <c r="H46" s="12">
         <v>7037635022</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E47" s="12">
+      <c r="E47" s="14">
         <v>22206</v>
       </c>
       <c r="F47" s="1">
@@ -2470,27 +2470,27 @@
       <c r="G47" s="1">
         <v>-77.087843000000007</v>
       </c>
-      <c r="H47" s="9">
+      <c r="H47" s="12">
         <v>7036711701</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E48" s="12">
+      <c r="E48" s="14">
         <v>22192</v>
       </c>
       <c r="F48" s="1">
@@ -2499,27 +2499,27 @@
       <c r="G48" s="1">
         <v>-77.288633000000004</v>
       </c>
-      <c r="H48" s="9">
+      <c r="H48" s="12">
         <v>7034910390</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E49" s="12">
+      <c r="E49" s="14">
         <v>22150</v>
       </c>
       <c r="F49" s="1">
@@ -2528,25 +2528,25 @@
       <c r="G49" s="1">
         <v>-77.193335000000005</v>
       </c>
-      <c r="H49" s="9">
+      <c r="H49" s="12">
         <v>7033374722</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="D50" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>176</v>
       </c>
       <c r="E50" s="15">
         <v>90034</v>
@@ -2557,27 +2557,27 @@
       <c r="G50" s="1">
         <v>-118.41441</v>
       </c>
-      <c r="H50" s="10">
+      <c r="H50" s="13">
         <v>3108366252</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B51" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="D51" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E51" s="13">
+        <v>174</v>
+      </c>
+      <c r="E51" s="16">
         <v>90210</v>
       </c>
       <c r="F51" s="1">
@@ -2586,56 +2586,56 @@
       <c r="G51" s="1">
         <v>-118.3997815</v>
       </c>
-      <c r="H51" s="10">
+      <c r="H51" s="13">
         <v>3103850880</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="D52" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E52" s="17">
+        <v>94105</v>
+      </c>
+      <c r="F52" s="11">
+        <v>37.785407499999998</v>
+      </c>
+      <c r="G52" s="11">
+        <v>-122.401301</v>
+      </c>
+      <c r="H52" s="13">
+        <v>4156854860</v>
+      </c>
+      <c r="I52" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="E52" s="16">
-        <v>94105</v>
-      </c>
-      <c r="F52" s="17">
-        <v>37.785407499999998</v>
-      </c>
-      <c r="G52" s="17">
-        <v>-122.401301</v>
-      </c>
-      <c r="H52" s="10">
-        <v>4156854860</v>
-      </c>
-      <c r="I52" s="7" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="D53" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E53" s="12">
+      <c r="E53" s="14">
         <v>60614</v>
       </c>
       <c r="F53" s="1">
@@ -2644,27 +2644,27 @@
       <c r="G53" s="1">
         <v>-87.650352699999999</v>
       </c>
-      <c r="H53" s="9">
+      <c r="H53" s="12">
         <v>3128670110</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="D54" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E54" s="12">
+        <v>174</v>
+      </c>
+      <c r="E54" s="14">
         <v>95030</v>
       </c>
       <c r="F54" s="1">
@@ -2673,27 +2673,27 @@
       <c r="G54" s="1">
         <v>-121.98302510000001</v>
       </c>
-      <c r="H54" s="9">
+      <c r="H54" s="12">
         <v>4083544330</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="D55" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E55" s="12">
+      <c r="E55" s="14">
         <v>10023</v>
       </c>
       <c r="F55" s="1">
@@ -2702,27 +2702,27 @@
       <c r="G55" s="1">
         <v>-73.985047800000004</v>
       </c>
-      <c r="H55" s="9">
+      <c r="H55" s="12">
         <v>2128249335</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E56" s="12">
+        <v>196</v>
+      </c>
+      <c r="E56" s="14">
         <v>10019</v>
       </c>
       <c r="F56" s="1">
@@ -2731,27 +2731,27 @@
       <c r="G56" s="1">
         <v>-73.983993499999997</v>
       </c>
-      <c r="H56" s="9">
+      <c r="H56" s="12">
         <v>2125541515</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E57" s="12">
+        <v>187</v>
+      </c>
+      <c r="E57" s="14">
         <v>60661</v>
       </c>
       <c r="F57" s="1">
@@ -2760,56 +2760,56 @@
       <c r="G57" s="1">
         <v>-87.647126299999996</v>
       </c>
-      <c r="H57" s="9">
+      <c r="H57" s="12">
         <v>3122349494</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E58" s="14">
+        <v>20003</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E58" s="12">
-        <v>20003</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="G58" s="1">
         <v>-76.998074000000003</v>
       </c>
-      <c r="H58" s="9">
+      <c r="H58" s="12">
         <v>2025957375</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E59" s="12">
+        <v>59</v>
+      </c>
+      <c r="E59" s="14">
         <v>20004</v>
       </c>
       <c r="F59" s="1">
@@ -2818,47 +2818,46 @@
       <c r="G59" s="1">
         <v>-77.025896000000003</v>
       </c>
-      <c r="H59" s="9">
+      <c r="H59" s="12">
         <v>2023930812</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I1" r:id="rId1"/>
-    <hyperlink ref="I2" r:id="rId2"/>
-    <hyperlink ref="I3" r:id="rId3"/>
-    <hyperlink ref="I4" r:id="rId4"/>
-    <hyperlink ref="I5" r:id="rId5"/>
-    <hyperlink ref="I6" r:id="rId6"/>
-    <hyperlink ref="I7" r:id="rId7"/>
-    <hyperlink ref="I8" r:id="rId8"/>
-    <hyperlink ref="I9" r:id="rId9"/>
-    <hyperlink ref="I10" r:id="rId10"/>
-    <hyperlink ref="I11" r:id="rId11"/>
-    <hyperlink ref="I12" r:id="rId12"/>
-    <hyperlink ref="I13" r:id="rId13"/>
-    <hyperlink ref="I14" r:id="rId14"/>
-    <hyperlink ref="I15" r:id="rId15"/>
-    <hyperlink ref="I16" r:id="rId16"/>
-    <hyperlink ref="I18" r:id="rId17"/>
-    <hyperlink ref="I19" r:id="rId18"/>
-    <hyperlink ref="I20" r:id="rId19"/>
-    <hyperlink ref="I21" r:id="rId20"/>
-    <hyperlink ref="I22" r:id="rId21"/>
-    <hyperlink ref="I23" r:id="rId22"/>
-    <hyperlink ref="I24" r:id="rId23"/>
-    <hyperlink ref="I25" r:id="rId24"/>
-    <hyperlink ref="I26" r:id="rId25"/>
-    <hyperlink ref="I27" r:id="rId26"/>
-    <hyperlink ref="I50" r:id="rId27"/>
-    <hyperlink ref="I51" r:id="rId28"/>
-    <hyperlink ref="I52" r:id="rId29"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
+    <hyperlink ref="I9" r:id="rId8"/>
+    <hyperlink ref="I10" r:id="rId9"/>
+    <hyperlink ref="I11" r:id="rId10"/>
+    <hyperlink ref="I12" r:id="rId11"/>
+    <hyperlink ref="I13" r:id="rId12"/>
+    <hyperlink ref="I14" r:id="rId13"/>
+    <hyperlink ref="I15" r:id="rId14"/>
+    <hyperlink ref="I16" r:id="rId15"/>
+    <hyperlink ref="I18" r:id="rId16"/>
+    <hyperlink ref="I19" r:id="rId17"/>
+    <hyperlink ref="I20" r:id="rId18"/>
+    <hyperlink ref="I21" r:id="rId19"/>
+    <hyperlink ref="I22" r:id="rId20"/>
+    <hyperlink ref="I23" r:id="rId21"/>
+    <hyperlink ref="I24" r:id="rId22"/>
+    <hyperlink ref="I25" r:id="rId23"/>
+    <hyperlink ref="I26" r:id="rId24"/>
+    <hyperlink ref="I27" r:id="rId25"/>
+    <hyperlink ref="I50" r:id="rId26"/>
+    <hyperlink ref="I51" r:id="rId27"/>
+    <hyperlink ref="I52" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
 

</xml_diff>